<commit_message>
bench on ss512 & ss1024
</commit_message>
<xml_diff>
--- a/BenchCDH.xlsx
+++ b/BenchCDH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnInsu\CryptoThesis\Commitment_Schemes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Desktop\UNINSU\CryptoThesis\Commitment_Schemes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9922A4-CA06-4637-B1D8-BD5673B3FF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B4AC59-0E02-422E-95D6-2BFAA1F8A371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>Based on CDH assumption</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>curve secp521r1</t>
+  </si>
+  <si>
+    <t>curve SS512</t>
+  </si>
+  <si>
+    <t>curve SS1024</t>
   </si>
 </sst>
 </file>
@@ -94,11 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -379,21 +383,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="102" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +411,7 @@
         <v>30.7499597072601</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -421,72 +425,72 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3.38625907897949E-3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>3.8309812545776298E-2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>3.53741645812988E-2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>0.746723651885986</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3.2393932342529201E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3.1945705413818299E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3.1628608703613199E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4.6272277832031198E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3.7841796875E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3.8797855377197201E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3.18026542663574E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3.19910049438476E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4.5380592346191398E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f>AVERAGE(A3:A12)</f>
         <v>3.6191701889038037E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -500,7 +504,7 @@
         <v>44.9191539287567</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -514,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>4.9306631088256801E-2</v>
       </c>
@@ -525,7 +529,7 @@
         <v>1.1031482219696001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -539,7 +543,7 @@
         <v>123.91518211364701</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -553,15 +557,93 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>6.4723730087280204E-2</v>
       </c>
       <c r="C21">
         <v>6.1742782592773403E-2</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
         <v>3.32143878936767</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>104.23850059509201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
+        <v>0.108036279678344</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.106045007705688</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.5685558319091699E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>201.82421469688401</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
+        <v>0.23519372940063399</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.23816847801208399</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3.3162832260131801E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bench with update method
</commit_message>
<xml_diff>
--- a/BenchCDH.xlsx
+++ b/BenchCDH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Desktop\UNINSU\CryptoThesis\Commitment_Schemes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B4AC59-0E02-422E-95D6-2BFAA1F8A371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CC9891-38F5-43C7-97BE-F5440ADE6FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
   <si>
     <t>Based on CDH assumption</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>curve SS1024</t>
+  </si>
+  <si>
+    <t>Update commit</t>
+  </si>
+  <si>
+    <t>Update proof</t>
   </si>
 </sst>
 </file>
@@ -383,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="102" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -395,6 +401,7 @@
     <col min="2" max="2" width="56.6640625" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="5" max="6" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -518,7 +525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>4.9306631088256801E-2</v>
       </c>
@@ -529,7 +536,7 @@
         <v>1.1031482219696001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -543,7 +550,7 @@
         <v>123.91518211364701</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -557,7 +564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>6.4723730087280204E-2</v>
       </c>
@@ -568,7 +575,7 @@
         <v>3.32143878936767</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -582,7 +589,7 @@
         <v>104.23850059509201</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -595,8 +602,14 @@
       <c r="D25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>0.108036279678344</v>
       </c>
@@ -606,8 +619,14 @@
       <c r="D26" s="1">
         <v>1.5685558319091699E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="1">
+        <v>1.5449523925781201E-4</v>
+      </c>
+      <c r="F26" s="1">
+        <v>4.55379486083984E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -621,7 +640,7 @@
         <v>201.82421469688401</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -634,8 +653,14 @@
       <c r="D29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>0.23519372940063399</v>
       </c>
@@ -644,6 +669,12 @@
       </c>
       <c r="D30" s="1">
         <v>3.3162832260131801E-2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>4.2510032653808502E-4</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1.0986328125E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>